<commit_message>
added background, text, basic boxes
</commit_message>
<xml_diff>
--- a/output/useroutput.xlsx
+++ b/output/useroutput.xlsx
@@ -389,7 +389,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1047</t>
+          <t>1033</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>100</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>71</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>69</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
redirected html, made flask load the html
</commit_message>
<xml_diff>
--- a/output/useroutput.xlsx
+++ b/output/useroutput.xlsx
@@ -389,7 +389,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1033</t>
+          <t>1008</t>
         </is>
       </c>
     </row>
@@ -404,7 +404,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>129</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>114</t>
         </is>
       </c>
     </row>
@@ -429,12 +429,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Kids See Ghosts</t>
+          <t>Kendrick Lamar</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>105</t>
         </is>
       </c>
     </row>
@@ -444,12 +444,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kendrick Lamar</t>
+          <t>Kids See Ghosts</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>98</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>94</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>73</t>
         </is>
       </c>
     </row>
@@ -504,12 +504,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Frank Ocean</t>
+          <t>JAY-Z</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>73</t>
         </is>
       </c>
     </row>
@@ -519,12 +519,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JAY-Z</t>
+          <t>Frank Ocean</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>72</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added working lastfm option inputs, general cleanup/optimization
</commit_message>
<xml_diff>
--- a/output/useroutput.xlsx
+++ b/output/useroutput.xlsx
@@ -389,7 +389,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1008</t>
+          <t>1027</t>
         </is>
       </c>
     </row>
@@ -404,7 +404,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>131</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>115</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>98</t>
+          <t>99</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>96</t>
         </is>
       </c>
     </row>
@@ -474,7 +474,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nas</t>
+          <t>JAY-Z</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -489,12 +489,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Chance the Rapper</t>
+          <t>Nas</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>75</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JAY-Z</t>
+          <t>Chance the Rapper</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">

</xml_diff>

<commit_message>
WORKING CHART + SMALL FIXES
</commit_message>
<xml_diff>
--- a/output/useroutput.xlsx
+++ b/output/useroutput.xlsx
@@ -389,7 +389,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1027</t>
+          <t>1038</t>
         </is>
       </c>
     </row>
@@ -404,7 +404,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>135</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>117</t>
         </is>
       </c>
     </row>
@@ -434,7 +434,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>108</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>100</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>97</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>76</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Nas</t>
+          <t>Chance the Rapper</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -504,12 +504,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Chance the Rapper</t>
+          <t>Nas</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>75</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>73</t>
         </is>
       </c>
     </row>

</xml_diff>